<commit_message>
Update cached digitize, classify, extract and export results in VB Small change to LoadDigitizationFromCache.xaml in VB
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Tests/Cache/ExportMergedDocuments_4-4.xlsx
+++ b/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Tests/Cache/ExportMergedDocuments_4-4.xlsx
@@ -82,61 +82,61 @@
     <x:t>Dough Zone</x:t>
   </x:si>
   <x:si>
-    <x:t>0.9415001</x:t>
+    <x:t>0.9359569</x:t>
   </x:si>
   <x:si>
     <x:t>1580 NW Gilman Blvd Suite 1 Issaquah WA, 98027</x:t>
   </x:si>
   <x:si>
-    <x:t>0.92402583</x:t>
+    <x:t>0.91714096</x:t>
   </x:si>
   <x:si>
     <x:t>425-427-5555</x:t>
   </x:si>
   <x:si>
-    <x:t>0.95184714</x:t>
+    <x:t>0.9687482</x:t>
   </x:si>
   <x:si>
     <x:t>2020-01-31</x:t>
   </x:si>
   <x:si>
-    <x:t>0.5879969</x:t>
+    <x:t>0.68830854</x:t>
   </x:si>
   <x:si>
     <x:t>0122</x:t>
   </x:si>
   <x:si>
-    <x:t>0.93218553</x:t>
+    <x:t>0.91500014</x:t>
   </x:si>
   <x:si>
     <x:t>food_meals</x:t>
   </x:si>
   <x:si>
-    <x:t>0.9168589</x:t>
+    <x:t>0.9930566</x:t>
   </x:si>
   <x:si>
     <x:t>9.34</x:t>
   </x:si>
   <x:si>
-    <x:t>0.92709297</x:t>
+    <x:t>0.95059097</x:t>
   </x:si>
   <x:si>
     <x:t>102.74</x:t>
   </x:si>
   <x:si>
-    <x:t>0.91842127</x:t>
+    <x:t>0.9489661</x:t>
   </x:si>
   <x:si>
     <x:t>USD</x:t>
   </x:si>
   <x:si>
-    <x:t>0.9848289</x:t>
+    <x:t>0.9461934</x:t>
   </x:si>
   <x:si>
     <x:t>table</x:t>
   </x:si>
   <x:si>
-    <x:t>0.6651519</x:t>
+    <x:t>0.6617088</x:t>
   </x:si>
   <x:si>
     <x:t>Description</x:t>
@@ -163,163 +163,163 @@
     <x:t>Line Amount - Confidence</x:t>
   </x:si>
   <x:si>
-    <x:t>green onion Pancakes (1)</x:t>
+    <x:t>green onion Pancakes NVIW@If (1)</x:t>
   </x:si>
   <x:si>
     <x:t>1</x:t>
   </x:si>
   <x:si>
-    <x:t>0.9535377</x:t>
+    <x:t>0.9654466</x:t>
   </x:si>
   <x:si>
     <x:t>2.95</x:t>
   </x:si>
   <x:si>
-    <x:t>0.95354986</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Pan Fried Leek Dumplings dNaY (2)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0.9253742</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0.95813227</x:t>
+    <x:t>0.96437496</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Pan Fried Leek Dumplings #j (2)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0.72182536</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0.92594826</x:t>
   </x:si>
   <x:si>
     <x:t>5.95</x:t>
   </x:si>
   <x:si>
-    <x:t>0.9508471</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Pork Xiao Long Bao(10)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0.89332026</x:t>
+    <x:t>0.9631321</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Pork Xiao Long Bao(10) MJINAME(10)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0.74614596</x:t>
   </x:si>
   <x:si>
     <x:t>2</x:t>
   </x:si>
   <x:si>
-    <x:t>0.9369251</x:t>
+    <x:t>0.8857973</x:t>
   </x:si>
   <x:si>
     <x:t>23.00</x:t>
   </x:si>
   <x:si>
-    <x:t>0.9455822</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Q-BAO (5) (5)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0.77509964</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0.9102243</x:t>
+    <x:t>0.97184485</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Q-BAO (5) HENE] (5)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0.8768804</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0.8922952</x:t>
   </x:si>
   <x:si>
     <x:t>11.25</x:t>
   </x:si>
   <x:si>
-    <x:t>0.93071574</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Chicken potstickers</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0.98189974</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0.9585857</x:t>
+    <x:t>0.96625626</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Chicken potstickers #ERJWAUA(6)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0.9518383</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0.92076415</x:t>
   </x:si>
   <x:si>
     <x:t>4.95</x:t>
   </x:si>
   <x:si>
-    <x:t>0.96048707</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Tomato Mushroom Steamed dumpli (6)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0.7809358</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0.93096113</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0.9678252</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Zucchini shrimp dumplings</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0.9730949</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0.9455834</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0.969649</x:t>
-  </x:si>
-  <x:si>
-    <x:t>beef stew nodle soup (Non Spicy Tb)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0.8166736</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0.9292481</x:t>
+    <x:t>0.9781219</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Tomato Mushroom Steamed dumpli ¿ (6)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0.929742</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0.93721306</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0.96639776</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Zucchini shrimp dumplings jJUUANUIC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0.97735536</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0.9401775</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0.9734021</x:t>
+  </x:si>
+  <x:si>
+    <x:t>beef stew nodle soup (Non Spicy 84pJ(T#)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0.8927655</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0.91823614</x:t>
   </x:si>
   <x:si>
     <x:t>8.95</x:t>
   </x:si>
   <x:si>
-    <x:t>0.96996593</x:t>
-  </x:si>
-  <x:si>
-    <x:t>dandan noodle</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0.97429997</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0.95896065</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0.97785324</x:t>
-  </x:si>
-  <x:si>
-    <x:t>banana naan bread</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0.9697557</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0.9477611</x:t>
+    <x:t>0.9591488</x:t>
+  </x:si>
+  <x:si>
+    <x:t>dandan noodle ttIÉÍ</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0.97385263</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0.909689</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0.9875826</x:t>
+  </x:si>
+  <x:si>
+    <x:t>banana naan bread EATA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0.9784949</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0.91455704</x:t>
   </x:si>
   <x:si>
     <x:t>10.50</x:t>
   </x:si>
   <x:si>
-    <x:t>0.98087126</x:t>
-  </x:si>
-  <x:si>
-    <x:t>house made plum juice</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0.9772749</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0.9415758</x:t>
+    <x:t>0.9884863</x:t>
+  </x:si>
+  <x:si>
+    <x:t>house made plum juice piumit</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0.9537653</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0.90424895</x:t>
   </x:si>
   <x:si>
     <x:t>9.00</x:t>
   </x:si>
   <x:si>
-    <x:t>0.94774336</x:t>
+    <x:t>0.9838298</x:t>
   </x:si>
   <x:si>
     <x:t>1.00</x:t>

</xml_diff>

<commit_message>
Update on Export.xaml Test Case
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Tests/Cache/ExportMergedDocuments_4-4.xlsx
+++ b/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Tests/Cache/ExportMergedDocuments_4-4.xlsx
@@ -91,7 +91,7 @@
     <x:t>Line Amount</x:t>
   </x:si>
   <x:si>
-    <x:t>green onion Pancakes ÂY/MAf (1)</x:t>
+    <x:t>green onion Pancakes MMt4AF (1)</x:t>
   </x:si>
   <x:si>
     <x:t>1</x:t>
@@ -100,13 +100,13 @@
     <x:t>2.95</x:t>
   </x:si>
   <x:si>
-    <x:t>Pan Fried Leek Dumplings #7 (2)</x:t>
+    <x:t>Pan Fried Leek Dumplings #8T (2)</x:t>
   </x:si>
   <x:si>
     <x:t>5.95</x:t>
   </x:si>
   <x:si>
-    <x:t>Pork Xiao Long Bao(10) AP])\$E(10)</x:t>
+    <x:t>Pork Xiao Long Bao(10) Ñ#P]]]NAÈ#Q(10)</x:t>
   </x:si>
   <x:si>
     <x:t>2</x:t>
@@ -115,40 +115,40 @@
     <x:t>23.00</x:t>
   </x:si>
   <x:si>
-    <x:t>Q-BA( (5) ĦEH'L (5)</x:t>
+    <x:t>Q-BA0) (5) MEÀE (5)</x:t>
   </x:si>
   <x:si>
     <x:t>11.25</x:t>
   </x:si>
   <x:si>
-    <x:t>Chicken potstickers HÈP]$9I5(6)</x:t>
+    <x:t>Chicken potstickers RÈP]]$/##5(6)</x:t>
   </x:si>
   <x:si>
     <x:t>4.95</x:t>
   </x:si>
   <x:si>
-    <x:t>Tomato Mushroom Steamed dumpli PEÅINABEEMKK (6)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Zucchini shrimp dumplings ĦJU]K</x:t>
-  </x:si>
-  <x:si>
-    <x:t>beef stew nodle soup (Non Spicy "H751PJ(74k)</x:t>
+    <x:t>Tomato Mushroom Steamed dumpli ₪ (6)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Zucchini shrimp dumplings j JJJ#tl6/5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>beef stew nodle soup (Non Spicy 25+ØJ(T#)</x:t>
   </x:si>
   <x:si>
     <x:t>8.95</x:t>
   </x:si>
   <x:si>
-    <x:t>dandan noodle</x:t>
-  </x:si>
-  <x:si>
-    <x:t>banana naan bread ¥</x:t>
+    <x:t>dandan noodle #/m</x:t>
+  </x:si>
+  <x:si>
+    <x:t>banana naan bread TATRAI</x:t>
   </x:si>
   <x:si>
     <x:t>10.50</x:t>
   </x:si>
   <x:si>
-    <x:t>house made plum juice ĚUNNT</x:t>
+    <x:t>house made plum juice</x:t>
   </x:si>
   <x:si>
     <x:t>9.00</x:t>

</xml_diff>

<commit_message>
fixed non-publishable package and updated packages
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Tests/Cache/ExportMergedDocuments_4-4.xlsx
+++ b/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Tests/Cache/ExportMergedDocuments_4-4.xlsx
@@ -91,7 +91,7 @@
     <x:t>Line Amount</x:t>
   </x:si>
   <x:si>
-    <x:t>green onion Pancakes MMt4AF (1)</x:t>
+    <x:t>green onion Pancakes ☐ (1)</x:t>
   </x:si>
   <x:si>
     <x:t>1</x:t>
@@ -100,13 +100,13 @@
     <x:t>2.95</x:t>
   </x:si>
   <x:si>
-    <x:t>Pan Fried Leek Dumplings #8T (2)</x:t>
+    <x:t>Pan Fried Leek Dumplings #T (2)</x:t>
   </x:si>
   <x:si>
     <x:t>5.95</x:t>
   </x:si>
   <x:si>
-    <x:t>Pork Xiao Long Bao(10) Ñ#P]]]NAÈ#Q(10)</x:t>
+    <x:t>Pork Xiao Long Bao(10) À#122E(10)</x:t>
   </x:si>
   <x:si>
     <x:t>2</x:t>
@@ -115,40 +115,40 @@
     <x:t>23.00</x:t>
   </x:si>
   <x:si>
-    <x:t>Q-BA0) (5) MEÀE (5)</x:t>
+    <x:t>Q-BAO (5) #E,EL (5)</x:t>
   </x:si>
   <x:si>
     <x:t>11.25</x:t>
   </x:si>
   <x:si>
-    <x:t>Chicken potstickers RÈP]]$/##5(6)</x:t>
+    <x:t>Chicken potstickers 3È#45(6)</x:t>
   </x:si>
   <x:si>
     <x:t>4.95</x:t>
   </x:si>
   <x:si>
-    <x:t>Tomato Mushroom Steamed dumpli ₪ (6)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Zucchini shrimp dumplings j JJJ#tl6/5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>beef stew nodle soup (Non Spicy 25+ØJ(T#)</x:t>
+    <x:t>Tomato Mushroom Steamed dumpli ptkINtA0 (6)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Zucchini shrimp dumplings #/2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>beef stew nodle soup (Non Spicy U4P11(7#)</x:t>
   </x:si>
   <x:si>
     <x:t>8.95</x:t>
   </x:si>
   <x:si>
-    <x:t>dandan noodle #/m</x:t>
-  </x:si>
-  <x:si>
-    <x:t>banana naan bread TATRAI</x:t>
+    <x:t>dandan noodle ##iE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>banana naan bread ZATRA</x:t>
   </x:si>
   <x:si>
     <x:t>10.50</x:t>
   </x:si>
   <x:si>
-    <x:t>house made plum juice</x:t>
+    <x:t>house made plum juice G$MSH+</x:t>
   </x:si>
   <x:si>
     <x:t>9.00</x:t>

</xml_diff>

<commit_message>
Windows VB - update RPA tests
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Tests/Cache/ExportMergedDocuments_4-4.xlsx
+++ b/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Tests/Cache/ExportMergedDocuments_4-4.xlsx
@@ -88,13 +88,13 @@
     <x:t>2.95</x:t>
   </x:si>
   <x:si>
-    <x:t>Pan Fried Leek Dumplings #AT (2)</x:t>
+    <x:t>Pan Fried Leek Dumplings IAT (2)</x:t>
   </x:si>
   <x:si>
     <x:t>5.95</x:t>
   </x:si>
   <x:si>
-    <x:t>Pork Xiao Long Bao(10) ¿*/ÅË#E(10)</x:t>
+    <x:t>Pork Xiao Long Bao(10) A¥R]J¿E(10)</x:t>
   </x:si>
   <x:si>
     <x:t>2</x:t>
@@ -103,40 +103,40 @@
     <x:t>23.00</x:t>
   </x:si>
   <x:si>
-    <x:t>Q-BAO (5) #NEJ (5)</x:t>
+    <x:t>Q-BAO (5) WEEL (5)</x:t>
   </x:si>
   <x:si>
     <x:t>11.25</x:t>
   </x:si>
   <x:si>
-    <x:t>Chicken potstickers *'ÈPJ$3N5(6)</x:t>
+    <x:t>Chicken potstickers KR$55(6)</x:t>
   </x:si>
   <x:si>
     <x:t>4.95</x:t>
   </x:si>
   <x:si>
-    <x:t>Tomato Mushroom Steamed dumpli PEATTAMAMKE (6)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Zucchini shrimp dumplings 7U#HA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>beef stew nodle soup (Non Spicy P¿#PJHE(T#)</x:t>
+    <x:t>Tomato Mushroom Steamed dumpli pEiAINABUNXA (6)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Zucchini shrimp dumplings A/LC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>beef stew nodle soup (Non Spicy 0H#4PJB(TY)</x:t>
   </x:si>
   <x:si>
     <x:t>8.95</x:t>
   </x:si>
   <x:si>
-    <x:t>dandan noodle #2H</x:t>
-  </x:si>
-  <x:si>
-    <x:t>banana naan bread EAA#</x:t>
+    <x:t>dandan noodle INCMM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>banana naan bread BATAI</x:t>
   </x:si>
   <x:si>
     <x:t>10.50</x:t>
   </x:si>
   <x:si>
-    <x:t>house made plum juice PUMgrt</x:t>
+    <x:t>house made plum juice</x:t>
   </x:si>
   <x:si>
     <x:t>9.00</x:t>

</xml_diff>